<commit_message>
Dev synchronization function. Add result area refresh.
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\backup-helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F87049F5-DCF2-4B0D-8BCA-9A3A2DF48B42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EEB44-D760-4DC6-8688-89925617DF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B83D038-40EF-4441-9110-D3708ACF505A}"/>
+    <workbookView xWindow="5580" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0B83D038-40EF-4441-9110-D3708ACF505A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -558,7 +558,7 @@
   <dimension ref="A1:BH26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AG30" sqref="AG30"/>
+      <selection activeCell="AW9" sqref="AW9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -876,6 +876,9 @@
       <c r="S8" s="5"/>
       <c r="T8" s="5"/>
       <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="X8" s="5"/>
       <c r="AC8" s="6" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
Dev: Truncate base path in result area.
</commit_message>
<xml_diff>
--- a/Layout.xlsx
+++ b/Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\backup-helper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41EEB44-D760-4DC6-8688-89925617DF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A48CC6A-9C27-40D0-8D83-26AC66C638F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5580" yWindow="4215" windowWidth="21600" windowHeight="11385" xr2:uid="{0B83D038-40EF-4441-9110-D3708ACF505A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0B83D038-40EF-4441-9110-D3708ACF505A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>Tip</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,14 @@
     <t>Process</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>Result explain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Path conversion notice</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -116,7 +124,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -189,6 +197,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -204,7 +218,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -239,6 +253,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -558,7 +575,7 @@
   <dimension ref="A1:BH26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AW9" sqref="AW9"/>
+      <selection activeCell="AS26" sqref="AS26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.125" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -850,6 +867,49 @@
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="C7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+      <c r="S7" s="12"/>
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="12"/>
+      <c r="W7" s="12"/>
+      <c r="X7" s="12"/>
+      <c r="Y7" s="12"/>
+      <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="12"/>
+      <c r="AJ7" s="12"/>
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="12"/>
+      <c r="AP7" s="12"/>
+      <c r="AQ7" s="12"/>
     </row>
     <row r="8" spans="1:60" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1003,7 +1063,9 @@
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>15</v>
+      </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="10"/>

</xml_diff>